<commit_message>
Worked on database deployment
</commit_message>
<xml_diff>
--- a/Docs/GanntChart.xlsx
+++ b/Docs/GanntChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286e2ff89c220aa4/Documents/University of Rochester/M2/DSCC483_DataScienceCapstone/URMCVenitaltorAllocation/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{89DAFC85-924A-4091-8922-94143E6F94D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A7D0FAD-5E9F-449E-ADAC-440BC5CA2F8E}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{89DAFC85-924A-4091-8922-94143E6F94D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{090393A3-F384-4343-B0D9-9563AE62F7A8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79D765E8-8A4C-40AE-A4DE-802E01F38C2A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -49,9 +49,6 @@
     <t>1. RSB Training</t>
   </si>
   <si>
-    <t>Derek, Nesli</t>
-  </si>
-  <si>
     <t>Week For</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Derek</t>
   </si>
   <si>
-    <t>Derek, Walter, Nesli</t>
-  </si>
-  <si>
     <t>3. Data Acquisition</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t>3.5 Develop Constraints</t>
-  </si>
-  <si>
-    <t>Derek,  Nesli</t>
   </si>
   <si>
     <t>3.6 Finalize Data Dictionary</t>
@@ -196,14 +187,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +513,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -539,23 +530,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -565,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>44605</v>
@@ -605,7 +596,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -614,62 +605,62 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>7</v>
+      <c r="A4" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -679,22 +670,22 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -704,49 +695,49 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -756,10 +747,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -768,11 +759,11 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -786,10 +777,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -803,10 +794,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>50</v>
@@ -819,8 +810,11 @@
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>27</v>
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
       </c>
       <c r="C19">
         <v>50</v>
@@ -834,35 +828,44 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
       </c>
       <c r="C20">
         <v>20</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
       </c>
       <c r="C22">
         <v>15</v>

</xml_diff>